<commit_message>
testing on more probs2
</commit_message>
<xml_diff>
--- a/examples/cpp/knapsack_hard/data/results.xlsx
+++ b/examples/cpp/knapsack_hard/data/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="301">
   <si>
     <t xml:space="preserve"> problem SENTO1.DAT</t>
   </si>
@@ -620,9 +620,6 @@
     <t>best weight target : 5567</t>
   </si>
   <si>
-    <t>algo: Swarm's Best</t>
-  </si>
-  <si>
     <t xml:space="preserve">best fly location: 1101(10.8586) 1010(5.49521) 0011(12.4168) 1011(12.8902) 0111(14.0023) 0110(5.80527) 0001(8.31215) 0110(5.92022) 1010(4.90714) 0000(0) </t>
   </si>
   <si>
@@ -888,6 +885,51 @@
   </si>
   <si>
     <t>best weight obtained : 6159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">best fly location: 0010(4.36785) 1001(9.4136) 0000(0) 1101(11.2202) 0110(5.59941) 0000(0) 1001(9.26979) 0100(2.21818) 0001(7.75693) 1000(1.26902) 1000(0.82573) 1110(7.24332) 0000(0) 1001(8.60651) 0010(4.45986) </t>
+  </si>
+  <si>
+    <t>fitness: 95.0317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knap 1: 4182 knap 2: 5977 knap 3: 4535 knap 4: 3660 knap 5: 4260 knap 6: 4828 knap 7: 3687 knap 8: 4839 knap 9: 5500 knap 10: 1672 knap 11: 4956 knap 12: 5568 knap 13: 3110 knap 14: 3878 knap 15: 5998 knap 16: 5475 knap 17: 2521 knap 18: 5221 knap 19: 4357 knap 20: 2337 knap 21: 5340 knap 22: 4893 knap 23: 4233 knap 24: 5810 knap 25: 5929 knap 26: 5818 knap 27: 4440 knap 28: 4564 knap 29: 3979 knap 30: 2363 </t>
+  </si>
+  <si>
+    <t>best weight obtained : 7662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">best fly location: 0101(10.2852) 1001(8.57139) 1000(1.36599) 1101(11.0179) 0100(2.03209) 0000(0) 1011(12.6928) 0100(2.12042) 0001(7.97002) 1000(0.943855) 0000(0) 0110(6.19531) 0000(0) 1001(9.16251) 0010(4.46302) </t>
+  </si>
+  <si>
+    <t>fitness: 134.968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knap 1: 4298 knap 2: 5158 knap 3: 5403 knap 4: 2888 knap 5: 5035 knap 6: 4793 knap 7: 3750 knap 8: 3355 knap 9: 5307 knap 10: 1657 knap 11: 3962 knap 12: 5043 knap 13: 3095 knap 14: 3901 knap 15: 5588 knap 16: 5778 knap 17: 2151 knap 18: 4633 knap 19: 4874 knap 20: 1598 knap 21: 4957 knap 22: 5758 knap 23: 4008 knap 24: 5717 knap 25: 5957 knap 26: 5966 knap 27: 3675 knap 28: 3153 knap 29: 3377 knap 30: 3471 </t>
+  </si>
+  <si>
+    <t>best weight obtained : 7636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">best fly location: 0010(3.88026) 1001(8.60732) 0000(0) 1101(10.9817) 0100(2.2577) 1000(1.29432) 1010(4.99314) 0110(5.99172) 0001(8.24405) 1000(1.22605) 0001(7.71258) 0110(5.68977) 0000(0) 1001(8.99) 1010(4.79893) </t>
+  </si>
+  <si>
+    <t>fitness: 195.455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knap 1: 4617 knap 2: 5838 knap 3: 5797 knap 4: 4027 knap 5: 5850 knap 6: 4771 knap 7: 5099 knap 8: 5358 knap 9: 5863 knap 10: 3361 knap 11: 4682 knap 12: 5287 knap 13: 4767 knap 14: 4188 knap 15: 5832 knap 16: 5335 knap 17: 2782 knap 18: 5323 knap 19: 4671 knap 20: 1789 knap 21: 4893 knap 22: 4501 knap 23: 4280 knap 24: 5748 knap 25: 5766 knap 26: 4922 knap 27: 3684 knap 28: 3864 knap 29: 3432 knap 30: 3296 </t>
+  </si>
+  <si>
+    <t>best weight obtained : 7611</t>
+  </si>
+  <si>
+    <t>algo: Best Neighbour, greed/safety ratio: 50</t>
+  </si>
+  <si>
+    <t>algo: Swarm's Best, greed/safety ratio: 10</t>
+  </si>
+  <si>
+    <t>algo: Best Neighbour, greed/safety ratio: 10</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY75"/>
+  <dimension ref="A1:AY111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1781,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>49</v>
@@ -1793,22 +1835,22 @@
         <v>191</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AA4" s="10"/>
       <c r="AB4" s="10"/>
@@ -1818,7 +1860,7 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>50</v>
@@ -1875,7 +1917,7 @@
         <v>50</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W5" s="8" t="s">
         <v>50</v>
@@ -1897,76 +1939,76 @@
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>197</v>
+        <v>299</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>299</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
@@ -1976,76 +2018,76 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="X7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA7" s="10"/>
       <c r="AB7" s="10"/>
@@ -2134,7 +2176,7 @@
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>53</v>
@@ -2188,22 +2230,22 @@
         <v>192</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z9" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
@@ -2267,22 +2309,22 @@
         <v>193</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X10" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z10" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
@@ -2425,22 +2467,22 @@
         <v>194</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X12" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA12" s="10"/>
       <c r="AB12" s="10"/>
@@ -2504,22 +2546,22 @@
         <v>195</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X13" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA13" s="10"/>
       <c r="AB13" s="10"/>
@@ -2583,22 +2625,22 @@
         <v>196</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="W14" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X14" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y14" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AA14" s="10"/>
       <c r="AB14" s="10"/>
@@ -2608,13 +2650,13 @@
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>72</v>
@@ -2635,10 +2677,10 @@
         <v>115</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>152</v>
@@ -2647,7 +2689,7 @@
         <v>161</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>176</v>
@@ -2656,28 +2698,28 @@
         <v>184</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z15" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AA15" s="10"/>
       <c r="AB15" s="10"/>
@@ -2687,7 +2729,7 @@
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>49</v>
@@ -2717,16 +2759,16 @@
         <v>191</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z16" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AA16" s="10"/>
       <c r="AB16" s="10"/>
@@ -2736,7 +2778,7 @@
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>140</v>
@@ -2784,39 +2826,39 @@
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="16" t="s">
-        <v>202</v>
+      <c r="C18" s="5" t="s">
+        <v>300</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="E18" s="15"/>
       <c r="L18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="5" t="s">
-        <v>197</v>
+      <c r="T18" s="19" t="s">
+        <v>299</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="8" t="s">
-        <v>202</v>
+        <v>300</v>
       </c>
       <c r="Z18" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA18" s="10"/>
       <c r="AB18" s="10"/>
@@ -2829,7 +2871,7 @@
         <v>51</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="10"/>
@@ -2839,33 +2881,33 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z19" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA19" s="10"/>
       <c r="AB19" s="10"/>
@@ -2924,7 +2966,7 @@
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>141</v>
@@ -2951,19 +2993,19 @@
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U21" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AA21" s="10"/>
       <c r="AB21" s="10"/>
@@ -3000,19 +3042,19 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U22" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AA22" s="10"/>
       <c r="AB22" s="10"/>
@@ -3098,19 +3140,19 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U24" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA24" s="10"/>
       <c r="AB24" s="10"/>
@@ -3147,19 +3189,19 @@
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U25" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
@@ -3199,16 +3241,16 @@
         <v>196</v>
       </c>
       <c r="U26" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AA26" s="10"/>
       <c r="AB26" s="10"/>
@@ -3218,10 +3260,10 @@
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>213</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -3231,15 +3273,15 @@
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -3248,13 +3290,13 @@
         <v>161</v>
       </c>
       <c r="U27" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z27" s="6" t="s">
         <v>184</v>
@@ -3325,7 +3367,7 @@
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
@@ -3342,7 +3384,7 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -3353,7 +3395,7 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="8" t="s">
-        <v>237</v>
+        <v>300</v>
       </c>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
@@ -3361,8 +3403,8 @@
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
-      <c r="T30" s="5" t="s">
-        <v>197</v>
+      <c r="T30" s="19" t="s">
+        <v>299</v>
       </c>
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
@@ -3379,7 +3421,7 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -3390,7 +3432,7 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="8" t="s">
-        <v>135</v>
+        <v>236</v>
       </c>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
@@ -3399,7 +3441,7 @@
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
       <c r="T31" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
@@ -3427,7 +3469,7 @@
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
       <c r="M32" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
@@ -3453,7 +3495,7 @@
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -3464,7 +3506,7 @@
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
       <c r="M33" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
@@ -3473,7 +3515,7 @@
       <c r="R33" s="10"/>
       <c r="S33" s="10"/>
       <c r="T33" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U33" s="10"/>
       <c r="V33" s="10"/>
@@ -3490,7 +3532,7 @@
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -3501,7 +3543,7 @@
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="8" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
@@ -3510,7 +3552,7 @@
       <c r="R34" s="10"/>
       <c r="S34" s="10"/>
       <c r="T34" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U34" s="10"/>
       <c r="V34" s="10"/>
@@ -3538,7 +3580,7 @@
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="8" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
@@ -3564,7 +3606,7 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -3575,7 +3617,7 @@
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
@@ -3584,7 +3626,7 @@
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
       <c r="T36" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U36" s="10"/>
       <c r="V36" s="10"/>
@@ -3601,7 +3643,7 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -3612,7 +3654,7 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="8" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
@@ -3621,7 +3663,7 @@
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U37" s="10"/>
       <c r="V37" s="10"/>
@@ -3633,7 +3675,7 @@
       <c r="AB37" s="10"/>
       <c r="AC37" s="10"/>
     </row>
-    <row r="38" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -3648,8 +3690,8 @@
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
-      <c r="M38" s="9" t="s">
-        <v>213</v>
+      <c r="M38" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
@@ -3675,7 +3717,7 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -3685,7 +3727,9 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
+      <c r="M39" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
@@ -3693,7 +3737,7 @@
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
       <c r="T39" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U39" s="10"/>
       <c r="V39" s="10"/>
@@ -3776,7 +3820,7 @@
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -3809,7 +3853,7 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -3842,7 +3886,7 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -3875,7 +3919,7 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -3908,7 +3952,7 @@
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -3974,7 +4018,7 @@
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
@@ -4007,7 +4051,7 @@
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -4073,7 +4117,7 @@
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -4139,7 +4183,7 @@
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -4172,7 +4216,7 @@
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
@@ -4205,7 +4249,7 @@
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
@@ -4238,7 +4282,7 @@
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
@@ -4271,7 +4315,7 @@
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
@@ -4304,7 +4348,7 @@
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
@@ -4370,7 +4414,7 @@
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
@@ -4403,7 +4447,7 @@
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
@@ -4469,7 +4513,7 @@
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
@@ -4509,27 +4553,27 @@
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D66" s="8" t="s">
-        <v>197</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D67" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D68" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D69" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D70" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.2">
@@ -4539,12 +4583,12 @@
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D72" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D73" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.2">
@@ -4554,7 +4598,187 @@
     </row>
     <row r="75" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D75" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D100" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D101" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D102" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D103" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D104" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D105" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D106" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D107" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D108" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D109" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D110" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>